<commit_message>
using long display id
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/cyanosource/plasmid/flanks.xlsx
+++ b/src/test/resources/ed/biordm/cyanosource/plasmid/flanks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NBeans\sbol-toolkit\src\main\resources\ed\biordm\cyanosource\plasmid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NBeans\sbol-toolkit\src\test\resources\ed\biordm\cyanosource\plasmid\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>0001_slr0611_left</t>
   </si>
@@ -60,12 +60,6 @@
     <t>ATGCCAAGGACTATGTACGGGCCATGTGGGCCATGTTGCAACAGGAACAGCCCGATGACTATGTGGTGGCCACGGGGGAAACCCACGAAGTGAAGGAATTTTTAGAAATTGCCTTTGGTTACGTCAACCTCAACTGGCAGAACTATGTGGCCTTTGATGAGCGCTATTTACGCCCCGCTGAAGTAGATTTATTAATCGGCGATCCGGCGAAAACCAAAGCCCAATTGGGCTGGGAACCCTCGGTTACCTTTACGGAATTAGTTCATTTAATGGTGGAGGCAGACTTAGCAGTCCTTGGTTTAACTTCTCCCAACCAGAGTGGACGAATCAAGGAGCTCATGGCCCAGGATATGGCCTTCATTCGGAGCCAAAATGGCCATGCCGTCGATTAAGCTTGGTTGAGCGTCTTAACTGTTGCCTCGATCAAAGTGTTTAACAACTAGCAATTTTCCCTGGCCTTCAAATGGTGGAGAATTTTATGGGCACAGTAAACCTAGGCAAATCCCTCCCTTAACTCAATATTTTCTTAACCAACC</t>
   </si>
   <si>
-    <t>name left</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Left flank sequence</t>
-  </si>
-  <si>
     <t>0001_slr0611_right</t>
   </si>
   <si>
@@ -93,10 +87,13 @@
     <t>GGTTGTCTTCCGCTGGATCACCTTTAGAACCTGTTTGAGAAGTTGAACTTTCGGCACATAATCCTTCCCAATCTCCCTTAAACGGGAAAGGTGGGGACTGTTGATAGTCGTTTTGAGACTTTTAAAACAGGCCTTTAAGCTGCTTCGGGTTGGATAAATCTGGTTTGTGAGTGAATGAAGTAAAAGCGCCCTGAGAATTTTGCCAAGTTTAGGTAAAATTTTTGGGGCATTTTTCCTGGCTGAAAATTTTTTGGCGGTGTGTTCGCCGCAATCATGGCAGATAATAGGGTTTGAAGGCTGATTAATCCCGCTGTTTCTATGTCTGATAATTTGACCGAACTCTCCCAACAACTCCATGATGCTTCAGAAAAAAAACAGTTGACGGCGATCGCCGCTTTGGCAGAAATGGGAGAAGGGGGCCAGGGAATATTACTCGATTATTTGGCCAAAAATGTCCCCCTAGAAAAGCCAGTGTTGGCGGTGGGTAACGTCTACCAAACCCTCCGGAATCTAGAACAGGAAACCATCACAACGCAACTCCA</t>
   </si>
   <si>
-    <t>name right</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Right flank sequence</t>
+    <t>display_id</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>left</t>
   </si>
 </sst>
 </file>
@@ -417,7 +414,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD3565"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,10 +424,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,7 +485,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD3565"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,47 +495,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>